<commit_message>
Added more comments in css file
</commit_message>
<xml_diff>
--- a/Documents/CST2120_ContributionSpreadsheet_FirstSubmission_draft1.xlsx.xlsx
+++ b/Documents/CST2120_ContributionSpreadsheet_FirstSubmission_draft1.xlsx.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_1519E771E0017C3DA0EC42A4B9DF9AADA1D17122" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE692F2F-6E8D-4275-9A39-B93EF51D7DCA}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_1519E771E0017C3DA0EC42A4B9DF9AADA1D17122" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D611CCE8-3CDE-4A4A-A1FB-518BEF711702}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -560,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -651,17 +651,17 @@
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="8">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="F7" s="8">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G7" s="8">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>IF(SUM(E7:F7)&lt;&gt;1,IF(SUM(E7:F7)=0, "Not implemented", "Error"),"Ok")</f>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -676,17 +676,17 @@
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="8">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="F8" s="8">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G8" s="8">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" ref="H8:H11" si="0">IF(SUM(E8:F8)&lt;&gt;1,IF(SUM(E8:F8)=0, "Not implemented", "Error"),"Ok")</f>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -701,17 +701,17 @@
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F9" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G9" s="8">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -726,17 +726,17 @@
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F10" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G10" s="8">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -751,17 +751,17 @@
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F11" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G11" s="8">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>